<commit_message>
chore: update ranked plots + SourceData (Fig2/EDFig4) and add CI workflows
</commit_message>
<xml_diff>
--- a/paper/journal_source_data/SourceData_EDFig4.xlsx
+++ b/paper/journal_source_data/SourceData_EDFig4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kfurudate/dev/LLM-PathwayCurator/paper/journal_source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EFBEE5-FBF7-1E48-8695-A3C389E8E644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D4D07C-9177-1548-A559-40D3CEB462B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="1000" windowWidth="24000" windowHeight="12840" xr2:uid="{30EB6BB9-ED82-374A-B580-C38CF118DFA7}"/>
+    <workbookView xWindow="8360" yWindow="1000" windowWidth="24000" windowHeight="12840" activeTab="5" xr2:uid="{30EB6BB9-ED82-374A-B580-C38CF118DFA7}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,13 @@
     <sheet name="EDFig4b_data" sheetId="10" r:id="rId3"/>
     <sheet name="EDFig4c_data" sheetId="11" r:id="rId4"/>
     <sheet name="EDFig4d_data" sheetId="12" r:id="rId5"/>
-    <sheet name="risk_coverage_full" sheetId="8" r:id="rId6"/>
+    <sheet name="EDFig4ef_data" sheetId="13" r:id="rId6"/>
+    <sheet name="risk_coverage_full" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDFig4a_data!$B$1:$B$106</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="366">
   <si>
     <t>Sheets</t>
   </si>
@@ -317,13 +318,838 @@
   </si>
   <si>
     <t>BEATAML_TP53_v1</t>
+  </si>
+  <si>
+    <t>・EDFig4ef_claims_ranked: Ranked claim shortlist used to render the BeatAML ranked views (from claims_ranked.tsv; see details below).</t>
+  </si>
+  <si>
+    <t>EDFig4ef_claims_ranked (panel e,f)</t>
+  </si>
+  <si>
+    <t>This sheet enables deterministic re-rendering of BeatAML ranked visualizations (packed/bars) from a single table.</t>
+  </si>
+  <si>
+    <t>Key derived quantity</t>
+  </si>
+  <si>
+    <t>Recommended columns (as-is from claims_ranked.tsv)</t>
+  </si>
+  <si>
+    <t>・identifiers: claim_id, module_id, term_uid, term_id, term_name</t>
+  </si>
+  <si>
+    <t>・decisions/annotations: decision, direction, direction_source</t>
+  </si>
+  <si>
+    <t>・components: stability, context_fit, evidence_strength (or evidence_strength_filled)</t>
+  </si>
+  <si>
+    <t>・ranking: utility_score, rank_global, module_utility_sum, module_rank, rank_in_module</t>
+  </si>
+  <si>
+    <t>・optional traceability: term_label, _join, score_source</t>
+  </si>
+  <si>
+    <t>・utility_score is the deterministic ranking score (e.g., evidence_strength_filled × stability × context_fit).</t>
+  </si>
+  <si>
+    <t>A figure-friendly ranked shortlist exported from the BeatAML run (claims_ranked.tsv).</t>
+  </si>
+  <si>
+    <t>claim_id</t>
+  </si>
+  <si>
+    <t>decision</t>
+  </si>
+  <si>
+    <t>module_id</t>
+  </si>
+  <si>
+    <t>term_uid</t>
+  </si>
+  <si>
+    <t>term_id</t>
+  </si>
+  <si>
+    <t>term_name</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>direction_source</t>
+  </si>
+  <si>
+    <t>stability</t>
+  </si>
+  <si>
+    <t>context_fit</t>
+  </si>
+  <si>
+    <t>evidence_strength</t>
+  </si>
+  <si>
+    <t>score_source</t>
+  </si>
+  <si>
+    <t>_join</t>
+  </si>
+  <si>
+    <t>term_label</t>
+  </si>
+  <si>
+    <t>evidence_strength_filled</t>
+  </si>
+  <si>
+    <t>utility_score</t>
+  </si>
+  <si>
+    <t>rank_global</t>
+  </si>
+  <si>
+    <t>module_utility_sum</t>
+  </si>
+  <si>
+    <t>module_rank</t>
+  </si>
+  <si>
+    <t>rank_in_module</t>
+  </si>
+  <si>
+    <t>c_9138ae157df8</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>M10c94544e295</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_G2M_CHECKPOINT</t>
+  </si>
+  <si>
+    <t>HALLMARK_G2M_CHECKPOINT</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>audit</t>
+  </si>
+  <si>
+    <t>HALLMARK_G2M_CHECKPOINT: HALLMARK_G2M_CHECKPOINT</t>
+  </si>
+  <si>
+    <t>c_276bff6c74a2</t>
+  </si>
+  <si>
+    <t>Mba84b3e143b8</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_EPITHELIAL_MESENCHYMAL_TRANSITION</t>
+  </si>
+  <si>
+    <t>HALLMARK_EPITHELIAL_MESENCHYMAL_TRANSITION</t>
+  </si>
+  <si>
+    <t>HALLMARK_EPITHELIAL_MESENCHYMAL_TRANSITION: HALLMARK_EPITHELIAL_MESENCHYMAL_TRANSITION</t>
+  </si>
+  <si>
+    <t>c_71ea86f16dad</t>
+  </si>
+  <si>
+    <t>Mde72f4c687b5</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_APICAL_JUNCTION</t>
+  </si>
+  <si>
+    <t>HALLMARK_APICAL_JUNCTION</t>
+  </si>
+  <si>
+    <t>HALLMARK_APICAL_JUNCTION: HALLMARK_APICAL_JUNCTION</t>
+  </si>
+  <si>
+    <t>c_8e844e5106a2</t>
+  </si>
+  <si>
+    <t>M9c70cf032c39</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_ESTROGEN_RESPONSE_LATE</t>
+  </si>
+  <si>
+    <t>HALLMARK_ESTROGEN_RESPONSE_LATE</t>
+  </si>
+  <si>
+    <t>HALLMARK_ESTROGEN_RESPONSE_LATE: HALLMARK_ESTROGEN_RESPONSE_LATE</t>
+  </si>
+  <si>
+    <t>c_cae0e751e647</t>
+  </si>
+  <si>
+    <t>M1f4f65ddbd4a</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_MTORC1_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_MTORC1_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_MTORC1_SIGNALING: HALLMARK_MTORC1_SIGNALING</t>
+  </si>
+  <si>
+    <t>c_364d36e8d358</t>
+  </si>
+  <si>
+    <t>M5ad8c232ffd3</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_INFLAMMATORY_RESPONSE</t>
+  </si>
+  <si>
+    <t>HALLMARK_INFLAMMATORY_RESPONSE</t>
+  </si>
+  <si>
+    <t>HALLMARK_INFLAMMATORY_RESPONSE: HALLMARK_INFLAMMATORY_RESPONSE</t>
+  </si>
+  <si>
+    <t>c_5df91a39807a</t>
+  </si>
+  <si>
+    <t>Mbabc22af87c9</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_SPERMATOGENESIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_SPERMATOGENESIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_SPERMATOGENESIS: HALLMARK_SPERMATOGENESIS</t>
+  </si>
+  <si>
+    <t>c_450cdc5cd834</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_TNFA_SIGNALING_VIA_NFKB</t>
+  </si>
+  <si>
+    <t>HALLMARK_TNFA_SIGNALING_VIA_NFKB</t>
+  </si>
+  <si>
+    <t>HALLMARK_TNFA_SIGNALING_VIA_NFKB: HALLMARK_TNFA_SIGNALING_VIA_NFKB</t>
+  </si>
+  <si>
+    <t>c_e2911daa664d</t>
+  </si>
+  <si>
+    <t>M4958bde29b6c</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_UV_RESPONSE_UP</t>
+  </si>
+  <si>
+    <t>HALLMARK_UV_RESPONSE_UP</t>
+  </si>
+  <si>
+    <t>HALLMARK_UV_RESPONSE_UP: HALLMARK_UV_RESPONSE_UP</t>
+  </si>
+  <si>
+    <t>c_e71b46ad58e7</t>
+  </si>
+  <si>
+    <t>M109e585f24ff</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_OXIDATIVE_PHOSPHORYLATION</t>
+  </si>
+  <si>
+    <t>HALLMARK_OXIDATIVE_PHOSPHORYLATION</t>
+  </si>
+  <si>
+    <t>down</t>
+  </si>
+  <si>
+    <t>HALLMARK_OXIDATIVE_PHOSPHORYLATION: HALLMARK_OXIDATIVE_PHOSPHORYLATION</t>
+  </si>
+  <si>
+    <t>c_b846c77d56ce</t>
+  </si>
+  <si>
+    <t>Mf7204a461589</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_UV_RESPONSE_DN</t>
+  </si>
+  <si>
+    <t>HALLMARK_UV_RESPONSE_DN</t>
+  </si>
+  <si>
+    <t>HALLMARK_UV_RESPONSE_DN: HALLMARK_UV_RESPONSE_DN</t>
+  </si>
+  <si>
+    <t>c_67a31e133375</t>
+  </si>
+  <si>
+    <t>Mc2675af46792</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_MYC_TARGETS_V2</t>
+  </si>
+  <si>
+    <t>HALLMARK_MYC_TARGETS_V2</t>
+  </si>
+  <si>
+    <t>HALLMARK_MYC_TARGETS_V2: HALLMARK_MYC_TARGETS_V2</t>
+  </si>
+  <si>
+    <t>c_1a89903f7256</t>
+  </si>
+  <si>
+    <t>M88cf93333440</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_APICAL_SURFACE</t>
+  </si>
+  <si>
+    <t>HALLMARK_APICAL_SURFACE</t>
+  </si>
+  <si>
+    <t>HALLMARK_APICAL_SURFACE: HALLMARK_APICAL_SURFACE</t>
+  </si>
+  <si>
+    <t>c_9e397d0e0e93</t>
+  </si>
+  <si>
+    <t>ABSTAIN</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_E2F_TARGETS</t>
+  </si>
+  <si>
+    <t>HALLMARK_E2F_TARGETS</t>
+  </si>
+  <si>
+    <t>HALLMARK_E2F_TARGETS: HALLMARK_E2F_TARGETS</t>
+  </si>
+  <si>
+    <t>c_964317476f4f</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_ESTROGEN_RESPONSE_EARLY</t>
+  </si>
+  <si>
+    <t>HALLMARK_ESTROGEN_RESPONSE_EARLY</t>
+  </si>
+  <si>
+    <t>HALLMARK_ESTROGEN_RESPONSE_EARLY: HALLMARK_ESTROGEN_RESPONSE_EARLY</t>
+  </si>
+  <si>
+    <t>c_47ab4d8c7f5c</t>
+  </si>
+  <si>
+    <t>Mf56ed728631d</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_KRAS_SIGNALING_DN</t>
+  </si>
+  <si>
+    <t>HALLMARK_KRAS_SIGNALING_DN</t>
+  </si>
+  <si>
+    <t>HALLMARK_KRAS_SIGNALING_DN: HALLMARK_KRAS_SIGNALING_DN</t>
+  </si>
+  <si>
+    <t>c_2a6dc80cfaf8</t>
+  </si>
+  <si>
+    <t>M030d0bf0c176</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_IL2_STAT5_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_IL2_STAT5_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_IL2_STAT5_SIGNALING: HALLMARK_IL2_STAT5_SIGNALING</t>
+  </si>
+  <si>
+    <t>c_50a5934c6cd1</t>
+  </si>
+  <si>
+    <t>M10c120fdec83</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_MYOGENESIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_MYOGENESIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_MYOGENESIS: HALLMARK_MYOGENESIS</t>
+  </si>
+  <si>
+    <t>c_207e0a204396</t>
+  </si>
+  <si>
+    <t>M001d3b4257ae</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_TGF_BETA_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_TGF_BETA_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_TGF_BETA_SIGNALING: HALLMARK_TGF_BETA_SIGNALING</t>
+  </si>
+  <si>
+    <t>c_400a1c2b0cda</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_MITOTIC_SPINDLE</t>
+  </si>
+  <si>
+    <t>HALLMARK_MITOTIC_SPINDLE</t>
+  </si>
+  <si>
+    <t>HALLMARK_MITOTIC_SPINDLE: HALLMARK_MITOTIC_SPINDLE</t>
+  </si>
+  <si>
+    <t>c_8a5f20f892f0</t>
+  </si>
+  <si>
+    <t>Mae5680496322</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_HEDGEHOG_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_HEDGEHOG_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_HEDGEHOG_SIGNALING: HALLMARK_HEDGEHOG_SIGNALING</t>
+  </si>
+  <si>
+    <t>c_fe0ca2ae33d0</t>
+  </si>
+  <si>
+    <t>M473fb04e1bf4</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_KRAS_SIGNALING_UP</t>
+  </si>
+  <si>
+    <t>HALLMARK_KRAS_SIGNALING_UP</t>
+  </si>
+  <si>
+    <t>HALLMARK_KRAS_SIGNALING_UP: HALLMARK_KRAS_SIGNALING_UP</t>
+  </si>
+  <si>
+    <t>c_7b052c54c7da</t>
+  </si>
+  <si>
+    <t>Mcf6b775ed5f3</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_ANDROGEN_RESPONSE</t>
+  </si>
+  <si>
+    <t>HALLMARK_ANDROGEN_RESPONSE</t>
+  </si>
+  <si>
+    <t>HALLMARK_ANDROGEN_RESPONSE: HALLMARK_ANDROGEN_RESPONSE</t>
+  </si>
+  <si>
+    <t>c_395e60655c4a</t>
+  </si>
+  <si>
+    <t>M88fc41364801</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_COAGULATION</t>
+  </si>
+  <si>
+    <t>HALLMARK_COAGULATION</t>
+  </si>
+  <si>
+    <t>HALLMARK_COAGULATION: HALLMARK_COAGULATION</t>
+  </si>
+  <si>
+    <t>c_cd057a97b9a0</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_IL6_JAK_STAT3_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_IL6_JAK_STAT3_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_IL6_JAK_STAT3_SIGNALING: HALLMARK_IL6_JAK_STAT3_SIGNALING</t>
+  </si>
+  <si>
+    <t>c_1145ca21bf67</t>
+  </si>
+  <si>
+    <t>M734186d89bdb</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_ANGIOGENESIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_ANGIOGENESIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_ANGIOGENESIS: HALLMARK_ANGIOGENESIS</t>
+  </si>
+  <si>
+    <t>c_100a570f5fc6</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_CHOLESTEROL_HOMEOSTASIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_CHOLESTEROL_HOMEOSTASIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_CHOLESTEROL_HOMEOSTASIS: HALLMARK_CHOLESTEROL_HOMEOSTASIS</t>
+  </si>
+  <si>
+    <t>c_cbb2cda65112</t>
+  </si>
+  <si>
+    <t>Mb6caa934d86e</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_HEME_METABOLISM</t>
+  </si>
+  <si>
+    <t>HALLMARK_HEME_METABOLISM</t>
+  </si>
+  <si>
+    <t>HALLMARK_HEME_METABOLISM: HALLMARK_HEME_METABOLISM</t>
+  </si>
+  <si>
+    <t>c_9b69058e35af</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_INTERFERON_ALPHA_RESPONSE</t>
+  </si>
+  <si>
+    <t>HALLMARK_INTERFERON_ALPHA_RESPONSE</t>
+  </si>
+  <si>
+    <t>HALLMARK_INTERFERON_ALPHA_RESPONSE: HALLMARK_INTERFERON_ALPHA_RESPONSE</t>
+  </si>
+  <si>
+    <t>c_2875af398278</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_COMPLEMENT</t>
+  </si>
+  <si>
+    <t>HALLMARK_COMPLEMENT</t>
+  </si>
+  <si>
+    <t>HALLMARK_COMPLEMENT: HALLMARK_COMPLEMENT</t>
+  </si>
+  <si>
+    <t>c_ab6344981456</t>
+  </si>
+  <si>
+    <t>M9e9aef27dc3d</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_MYC_TARGETS_V1</t>
+  </si>
+  <si>
+    <t>HALLMARK_MYC_TARGETS_V1</t>
+  </si>
+  <si>
+    <t>HALLMARK_MYC_TARGETS_V1: HALLMARK_MYC_TARGETS_V1</t>
+  </si>
+  <si>
+    <t>c_90d5c57c0bd3</t>
+  </si>
+  <si>
+    <t>Mf49fdc9ffbda</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_APOPTOSIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_APOPTOSIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_APOPTOSIS: HALLMARK_APOPTOSIS</t>
+  </si>
+  <si>
+    <t>c_a82594b21128</t>
+  </si>
+  <si>
+    <t>M76d2b450cd9b</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_WNT_BETA_CATENIN_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_WNT_BETA_CATENIN_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_WNT_BETA_CATENIN_SIGNALING: HALLMARK_WNT_BETA_CATENIN_SIGNALING</t>
+  </si>
+  <si>
+    <t>c_0625b0d0790b</t>
+  </si>
+  <si>
+    <t>Me7f4ca4a1479</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_UNFOLDED_PROTEIN_RESPONSE</t>
+  </si>
+  <si>
+    <t>HALLMARK_UNFOLDED_PROTEIN_RESPONSE</t>
+  </si>
+  <si>
+    <t>HALLMARK_UNFOLDED_PROTEIN_RESPONSE: HALLMARK_UNFOLDED_PROTEIN_RESPONSE</t>
+  </si>
+  <si>
+    <t>c_732459afdaa3</t>
+  </si>
+  <si>
+    <t>M102c62cc5b82</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_BILE_ACID_METABOLISM</t>
+  </si>
+  <si>
+    <t>HALLMARK_BILE_ACID_METABOLISM</t>
+  </si>
+  <si>
+    <t>HALLMARK_BILE_ACID_METABOLISM: HALLMARK_BILE_ACID_METABOLISM</t>
+  </si>
+  <si>
+    <t>c_98bc292b0cca</t>
+  </si>
+  <si>
+    <t>Me9bf4742b516</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_PI3K_AKT_MTOR_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_PI3K_AKT_MTOR_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_PI3K_AKT_MTOR_SIGNALING: HALLMARK_PI3K_AKT_MTOR_SIGNALING</t>
+  </si>
+  <si>
+    <t>c_c4ef246736df</t>
+  </si>
+  <si>
+    <t>M63598010daa2</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_FATTY_ACID_METABOLISM</t>
+  </si>
+  <si>
+    <t>HALLMARK_FATTY_ACID_METABOLISM</t>
+  </si>
+  <si>
+    <t>HALLMARK_FATTY_ACID_METABOLISM: HALLMARK_FATTY_ACID_METABOLISM</t>
+  </si>
+  <si>
+    <t>c_6fe04c32a662</t>
+  </si>
+  <si>
+    <t>Mda6326f0d7bf</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_PROTEIN_SECRETION</t>
+  </si>
+  <si>
+    <t>HALLMARK_PROTEIN_SECRETION</t>
+  </si>
+  <si>
+    <t>HALLMARK_PROTEIN_SECRETION: HALLMARK_PROTEIN_SECRETION</t>
+  </si>
+  <si>
+    <t>c_ce666bdd9f29</t>
+  </si>
+  <si>
+    <t>Mdf6607068867</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_ADIPOGENESIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_ADIPOGENESIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_ADIPOGENESIS: HALLMARK_ADIPOGENESIS</t>
+  </si>
+  <si>
+    <t>c_57c3badb424e</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_INTERFERON_GAMMA_RESPONSE</t>
+  </si>
+  <si>
+    <t>HALLMARK_INTERFERON_GAMMA_RESPONSE</t>
+  </si>
+  <si>
+    <t>HALLMARK_INTERFERON_GAMMA_RESPONSE: HALLMARK_INTERFERON_GAMMA_RESPONSE</t>
+  </si>
+  <si>
+    <t>c_a09822cead85</t>
+  </si>
+  <si>
+    <t>M8613e37e866b</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_XENOBIOTIC_METABOLISM</t>
+  </si>
+  <si>
+    <t>HALLMARK_XENOBIOTIC_METABOLISM</t>
+  </si>
+  <si>
+    <t>HALLMARK_XENOBIOTIC_METABOLISM: HALLMARK_XENOBIOTIC_METABOLISM</t>
+  </si>
+  <si>
+    <t>c_2ddb1c805b31</t>
+  </si>
+  <si>
+    <t>M75d8d1af5bcb</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_P53_PATHWAY</t>
+  </si>
+  <si>
+    <t>HALLMARK_P53_PATHWAY</t>
+  </si>
+  <si>
+    <t>HALLMARK_P53_PATHWAY: HALLMARK_P53_PATHWAY</t>
+  </si>
+  <si>
+    <t>c_941e4d647100</t>
+  </si>
+  <si>
+    <t>M3f3292a3d432</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_DNA_REPAIR</t>
+  </si>
+  <si>
+    <t>HALLMARK_DNA_REPAIR</t>
+  </si>
+  <si>
+    <t>HALLMARK_DNA_REPAIR: HALLMARK_DNA_REPAIR</t>
+  </si>
+  <si>
+    <t>c_af19760478e6</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_PEROXISOME</t>
+  </si>
+  <si>
+    <t>HALLMARK_PEROXISOME</t>
+  </si>
+  <si>
+    <t>HALLMARK_PEROXISOME: HALLMARK_PEROXISOME</t>
+  </si>
+  <si>
+    <t>c_455dba37be71</t>
+  </si>
+  <si>
+    <t>M2fbb6d7ec279</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_GLYCOLYSIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_GLYCOLYSIS</t>
+  </si>
+  <si>
+    <t>HALLMARK_GLYCOLYSIS: HALLMARK_GLYCOLYSIS</t>
+  </si>
+  <si>
+    <t>c_5ad9b02b81c9</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_NOTCH_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_NOTCH_SIGNALING</t>
+  </si>
+  <si>
+    <t>HALLMARK_NOTCH_SIGNALING: HALLMARK_NOTCH_SIGNALING</t>
+  </si>
+  <si>
+    <t>c_640cd3fdde66</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_ALLOGRAFT_REJECTION</t>
+  </si>
+  <si>
+    <t>HALLMARK_ALLOGRAFT_REJECTION</t>
+  </si>
+  <si>
+    <t>HALLMARK_ALLOGRAFT_REJECTION: HALLMARK_ALLOGRAFT_REJECTION</t>
+  </si>
+  <si>
+    <t>c_795815b409e8</t>
+  </si>
+  <si>
+    <t>M066e297c8710</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_REACTIVE_OXYGEN_SPECIES_PATHWAY</t>
+  </si>
+  <si>
+    <t>HALLMARK_REACTIVE_OXYGEN_SPECIES_PATHWAY</t>
+  </si>
+  <si>
+    <t>HALLMARK_REACTIVE_OXYGEN_SPECIES_PATHWAY: HALLMARK_REACTIVE_OXYGEN_SPECIES_PATHWAY</t>
+  </si>
+  <si>
+    <t>c_cf13126e115b</t>
+  </si>
+  <si>
+    <t>M04098975cc06</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_PANCREAS_BETA_CELLS</t>
+  </si>
+  <si>
+    <t>HALLMARK_PANCREAS_BETA_CELLS</t>
+  </si>
+  <si>
+    <t>HALLMARK_PANCREAS_BETA_CELLS: HALLMARK_PANCREAS_BETA_CELLS</t>
+  </si>
+  <si>
+    <t>c_36d7fb1fbdc1</t>
+  </si>
+  <si>
+    <t>fgsea_msigdb_H_ensembl:HALLMARK_HYPOXIA</t>
+  </si>
+  <si>
+    <t>HALLMARK_HYPOXIA</t>
+  </si>
+  <si>
+    <t>HALLMARK_HYPOXIA: HALLMARK_HYPOXIA</t>
+  </si>
+  <si>
+    <t>-LOG10(qval)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -365,6 +1191,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -387,12 +1220,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -728,9 +1563,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9673388-7D5D-2945-93B6-903C0FEE4E1B}">
-  <dimension ref="A1:A70"/>
+  <dimension ref="A1:A84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -760,278 +1595,338 @@
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
+    <row r="26" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>14</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>3</v>
+      <c r="A68" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1041,7 +1936,8 @@
     <hyperlink ref="A8" location="EDFig4b_data!A1" display="・EDFig4b_abstain_vs_tau: ABSTAIN rate across τ for BeatAML (panel b)." xr:uid="{8B3BAE3E-E67A-0E4B-A556-776DB679F891}"/>
     <hyperlink ref="A9" location="EDFig4c_data!A1" display="・EDFig4c_pass_vs_human_risk: PASS rate vs human non-accept risk (BeatAML; panel c)." xr:uid="{294CC777-1F5E-214E-BFDC-6C957B425551}"/>
     <hyperlink ref="A10" location="EDFig4d_data!A1" display="・EDFig4d_abstain_reasons: ABSTAIN reason-code composition (BeatAML; panel d)." xr:uid="{47A86D76-D053-3D4C-981A-A376946E30AE}"/>
-    <hyperlink ref="A11" location="risk_coverage_full!A1" display="・risk_coverage_full: Full exported table used for plotting (risk_coverage.tsv; optional “complete view”)." xr:uid="{1E45B6CF-2341-3140-BF16-9380A8B7A8FE}"/>
+    <hyperlink ref="A12" location="risk_coverage_full!A1" display="・risk_coverage_full: Full exported table used for plotting (risk_coverage.tsv; optional “complete view”)." xr:uid="{1E45B6CF-2341-3140-BF16-9380A8B7A8FE}"/>
+    <hyperlink ref="A11" location="EDFig4ef_data!A1" display="・EDFig4ef_claims_ranked: Ranked claim shortlist used to render the BeatAML ranked views (from claims_ranked.tsv; see details below)." xr:uid="{7FA1622E-6025-E647-853D-4357C1327DEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3062,6 +3958,3186 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F00334-8E8A-2842-BB24-93AE8720C55F}">
+  <dimension ref="A1:T51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="N21" sqref="M21:N51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>119</v>
+      </c>
+      <c r="R1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S1" t="s">
+        <v>121</v>
+      </c>
+      <c r="T1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.88948940419623501</v>
+      </c>
+      <c r="K2">
+        <v>32.917841429395999</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M2" t="s">
+        <v>127</v>
+      </c>
+      <c r="N2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O2">
+        <v>32.917841429395999</v>
+      </c>
+      <c r="P2">
+        <v>29.280071160459599</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>33.541256571738799</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.82881077240639001</v>
+      </c>
+      <c r="K3">
+        <v>11.959474735037499</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N3" t="s">
+        <v>135</v>
+      </c>
+      <c r="O3">
+        <v>11.959474735037499</v>
+      </c>
+      <c r="P3">
+        <v>9.91214149272116</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>9.91214149272116</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.74647861248021796</v>
+      </c>
+      <c r="K4">
+        <v>7.0045766339754101</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M4" t="s">
+        <v>139</v>
+      </c>
+      <c r="N4" t="s">
+        <v>140</v>
+      </c>
+      <c r="O4">
+        <v>7.0045766339754101</v>
+      </c>
+      <c r="P4">
+        <v>5.2287666467413203</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4">
+        <v>5.2287666467413203</v>
+      </c>
+      <c r="S4">
+        <v>6</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.37397308208427699</v>
+      </c>
+      <c r="K5">
+        <v>12.3454787531698</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M5" t="s">
+        <v>144</v>
+      </c>
+      <c r="N5" t="s">
+        <v>145</v>
+      </c>
+      <c r="O5">
+        <v>12.3454787531698</v>
+      </c>
+      <c r="P5">
+        <v>4.6168767391288803</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5">
+        <v>6.9947954003983899</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" t="s">
+        <v>128</v>
+      </c>
+      <c r="H6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0.60319121543865695</v>
+      </c>
+      <c r="K6">
+        <v>7.3426509839008096</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M6" t="s">
+        <v>149</v>
+      </c>
+      <c r="N6" t="s">
+        <v>150</v>
+      </c>
+      <c r="O6">
+        <v>7.3426509839008096</v>
+      </c>
+      <c r="P6">
+        <v>4.4290225715209797</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>5.5567430041196104</v>
+      </c>
+      <c r="S6">
+        <v>5</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0.56207923549392302</v>
+      </c>
+      <c r="K7">
+        <v>7.4335317494593403</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M7" t="s">
+        <v>154</v>
+      </c>
+      <c r="N7" t="s">
+        <v>155</v>
+      </c>
+      <c r="O7">
+        <v>7.4335317494593403</v>
+      </c>
+      <c r="P7">
+        <v>4.17823384275591</v>
+      </c>
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <v>10.112949522140299</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" t="s">
+        <v>129</v>
+      </c>
+      <c r="I8">
+        <v>0.984375</v>
+      </c>
+      <c r="J8">
+        <v>0.73430938974837001</v>
+      </c>
+      <c r="K8">
+        <v>5.7057426757747196</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M8" t="s">
+        <v>159</v>
+      </c>
+      <c r="N8" t="s">
+        <v>160</v>
+      </c>
+      <c r="O8">
+        <v>5.7057426757747196</v>
+      </c>
+      <c r="P8">
+        <v>4.1243151032107903</v>
+      </c>
+      <c r="Q8">
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>4.1243151032107903</v>
+      </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0.75682556816603697</v>
+      </c>
+      <c r="K9">
+        <v>4.9834649591105604</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M9" t="s">
+        <v>163</v>
+      </c>
+      <c r="N9" t="s">
+        <v>164</v>
+      </c>
+      <c r="O9">
+        <v>4.9834649591105604</v>
+      </c>
+      <c r="P9">
+        <v>3.7716136991143898</v>
+      </c>
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9">
+        <v>10.112949522140299</v>
+      </c>
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" t="s">
+        <v>168</v>
+      </c>
+      <c r="G10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10">
+        <v>0.984375</v>
+      </c>
+      <c r="J10">
+        <v>0.78454422768911503</v>
+      </c>
+      <c r="K10">
+        <v>4.7747059180534004</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M10" t="s">
+        <v>168</v>
+      </c>
+      <c r="N10" t="s">
+        <v>169</v>
+      </c>
+      <c r="O10">
+        <v>4.7747059180534004</v>
+      </c>
+      <c r="P10">
+        <v>3.6874372174387</v>
+      </c>
+      <c r="Q10">
+        <v>9</v>
+      </c>
+      <c r="R10">
+        <v>3.6874372174387</v>
+      </c>
+      <c r="S10">
+        <v>8</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" t="s">
+        <v>173</v>
+      </c>
+      <c r="F11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G11" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0.38683680723877401</v>
+      </c>
+      <c r="K11">
+        <v>9.1543440649538699</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M11" t="s">
+        <v>173</v>
+      </c>
+      <c r="N11" t="s">
+        <v>175</v>
+      </c>
+      <c r="O11">
+        <v>9.1543440649538699</v>
+      </c>
+      <c r="P11">
+        <v>3.5412372304519799</v>
+      </c>
+      <c r="Q11">
+        <v>10</v>
+      </c>
+      <c r="R11">
+        <v>3.5412372304519799</v>
+      </c>
+      <c r="S11">
+        <v>9</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D12" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" t="s">
+        <v>179</v>
+      </c>
+      <c r="G12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H12" t="s">
+        <v>129</v>
+      </c>
+      <c r="I12">
+        <v>0.984375</v>
+      </c>
+      <c r="J12">
+        <v>0.53897952258538095</v>
+      </c>
+      <c r="K12">
+        <v>6.6154232730936799</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M12" t="s">
+        <v>179</v>
+      </c>
+      <c r="N12" t="s">
+        <v>180</v>
+      </c>
+      <c r="O12">
+        <v>6.6154232730936799</v>
+      </c>
+      <c r="P12">
+        <v>3.5098655262223799</v>
+      </c>
+      <c r="Q12">
+        <v>11</v>
+      </c>
+      <c r="R12">
+        <v>3.5098655262223799</v>
+      </c>
+      <c r="S12">
+        <v>10</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G13" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" t="s">
+        <v>129</v>
+      </c>
+      <c r="I13">
+        <v>0.921875</v>
+      </c>
+      <c r="J13">
+        <v>0.84942088672323401</v>
+      </c>
+      <c r="K13">
+        <v>3.6013953222946902</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M13" t="s">
+        <v>184</v>
+      </c>
+      <c r="N13" t="s">
+        <v>185</v>
+      </c>
+      <c r="O13">
+        <v>3.6013953222946902</v>
+      </c>
+      <c r="P13">
+        <v>2.8201081887213002</v>
+      </c>
+      <c r="Q13">
+        <v>12</v>
+      </c>
+      <c r="R13">
+        <v>2.8201081887213002</v>
+      </c>
+      <c r="S13">
+        <v>11</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E14" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" t="s">
+        <v>189</v>
+      </c>
+      <c r="G14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14">
+        <v>0.953125</v>
+      </c>
+      <c r="J14">
+        <v>0.86120487231771303</v>
+      </c>
+      <c r="K14">
+        <v>3.36038636918168</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M14" t="s">
+        <v>189</v>
+      </c>
+      <c r="N14" t="s">
+        <v>190</v>
+      </c>
+      <c r="O14">
+        <v>3.36038636918168</v>
+      </c>
+      <c r="P14">
+        <v>2.7583257492901101</v>
+      </c>
+      <c r="Q14">
+        <v>13</v>
+      </c>
+      <c r="R14">
+        <v>2.7583257492901101</v>
+      </c>
+      <c r="S14">
+        <v>12</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" t="s">
+        <v>193</v>
+      </c>
+      <c r="E15" t="s">
+        <v>194</v>
+      </c>
+      <c r="F15" t="s">
+        <v>194</v>
+      </c>
+      <c r="G15" t="s">
+        <v>128</v>
+      </c>
+      <c r="H15" t="s">
+        <v>129</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>7.3902968403484801E-2</v>
+      </c>
+      <c r="K15">
+        <v>34.913769559571797</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M15" t="s">
+        <v>194</v>
+      </c>
+      <c r="N15" t="s">
+        <v>195</v>
+      </c>
+      <c r="O15">
+        <v>34.913769559571797</v>
+      </c>
+      <c r="P15">
+        <v>2.58023120860758</v>
+      </c>
+      <c r="Q15">
+        <v>14</v>
+      </c>
+      <c r="R15">
+        <v>33.541256571738799</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H16" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16">
+        <v>0.984375</v>
+      </c>
+      <c r="J16">
+        <v>0.29350495386588499</v>
+      </c>
+      <c r="K16">
+        <v>8.2304007823608991</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M16" t="s">
+        <v>198</v>
+      </c>
+      <c r="N16" t="s">
+        <v>199</v>
+      </c>
+      <c r="O16">
+        <v>8.2304007823608991</v>
+      </c>
+      <c r="P16">
+        <v>2.37791866126951</v>
+      </c>
+      <c r="Q16">
+        <v>15</v>
+      </c>
+      <c r="R16">
+        <v>6.9947954003983899</v>
+      </c>
+      <c r="S16">
+        <v>4</v>
+      </c>
+      <c r="T16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" t="s">
+        <v>203</v>
+      </c>
+      <c r="F17" t="s">
+        <v>203</v>
+      </c>
+      <c r="G17" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0.63053391140098902</v>
+      </c>
+      <c r="K17">
+        <v>3.6835916290818802</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M17" t="s">
+        <v>203</v>
+      </c>
+      <c r="N17" t="s">
+        <v>204</v>
+      </c>
+      <c r="O17">
+        <v>3.6835916290818802</v>
+      </c>
+      <c r="P17">
+        <v>2.3226294378889398</v>
+      </c>
+      <c r="Q17">
+        <v>16</v>
+      </c>
+      <c r="R17">
+        <v>2.3226294378889398</v>
+      </c>
+      <c r="S17">
+        <v>13</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E18" t="s">
+        <v>208</v>
+      </c>
+      <c r="F18" t="s">
+        <v>208</v>
+      </c>
+      <c r="G18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" t="s">
+        <v>129</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0.312324455221834</v>
+      </c>
+      <c r="K18">
+        <v>5.9156415413842298</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M18" t="s">
+        <v>208</v>
+      </c>
+      <c r="N18" t="s">
+        <v>209</v>
+      </c>
+      <c r="O18">
+        <v>5.9156415413842298</v>
+      </c>
+      <c r="P18">
+        <v>1.8475995217004799</v>
+      </c>
+      <c r="Q18">
+        <v>17</v>
+      </c>
+      <c r="R18">
+        <v>1.8475995217004799</v>
+      </c>
+      <c r="S18">
+        <v>15</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>210</v>
+      </c>
+      <c r="B19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" t="s">
+        <v>212</v>
+      </c>
+      <c r="E19" t="s">
+        <v>213</v>
+      </c>
+      <c r="F19" t="s">
+        <v>213</v>
+      </c>
+      <c r="G19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" t="s">
+        <v>129</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0.42232234658811701</v>
+      </c>
+      <c r="K19">
+        <v>4.0919102961248299</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M19" t="s">
+        <v>213</v>
+      </c>
+      <c r="N19" t="s">
+        <v>214</v>
+      </c>
+      <c r="O19">
+        <v>4.0919102961248299</v>
+      </c>
+      <c r="P19">
+        <v>1.72810515828751</v>
+      </c>
+      <c r="Q19">
+        <v>18</v>
+      </c>
+      <c r="R19">
+        <v>1.72810515828751</v>
+      </c>
+      <c r="S19">
+        <v>16</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" t="s">
+        <v>216</v>
+      </c>
+      <c r="D20" t="s">
+        <v>217</v>
+      </c>
+      <c r="E20" t="s">
+        <v>218</v>
+      </c>
+      <c r="F20" t="s">
+        <v>218</v>
+      </c>
+      <c r="G20" t="s">
+        <v>128</v>
+      </c>
+      <c r="H20" t="s">
+        <v>129</v>
+      </c>
+      <c r="I20">
+        <v>0.921875</v>
+      </c>
+      <c r="J20">
+        <v>0.78725917749365404</v>
+      </c>
+      <c r="K20">
+        <v>2.3514223871352602</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M20" t="s">
+        <v>218</v>
+      </c>
+      <c r="N20" t="s">
+        <v>219</v>
+      </c>
+      <c r="O20">
+        <v>2.3514223871352602</v>
+      </c>
+      <c r="P20">
+        <v>1.7065555064334399</v>
+      </c>
+      <c r="Q20">
+        <v>19</v>
+      </c>
+      <c r="R20">
+        <v>1.7065555064334399</v>
+      </c>
+      <c r="S20">
+        <v>17</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>220</v>
+      </c>
+      <c r="B21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" t="s">
+        <v>221</v>
+      </c>
+      <c r="E21" t="s">
+        <v>222</v>
+      </c>
+      <c r="F21" t="s">
+        <v>222</v>
+      </c>
+      <c r="G21" t="s">
+        <v>128</v>
+      </c>
+      <c r="H21" t="s">
+        <v>129</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0.13489061330105401</v>
+      </c>
+      <c r="K21">
+        <v>12.4616099040189</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M21" t="s">
+        <v>222</v>
+      </c>
+      <c r="N21" t="s">
+        <v>223</v>
+      </c>
+      <c r="O21">
+        <v>12.4616099040189</v>
+      </c>
+      <c r="P21">
+        <v>1.6809542026716</v>
+      </c>
+      <c r="Q21">
+        <v>20</v>
+      </c>
+      <c r="R21">
+        <v>33.541256571738799</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>224</v>
+      </c>
+      <c r="B22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" t="s">
+        <v>225</v>
+      </c>
+      <c r="D22" t="s">
+        <v>226</v>
+      </c>
+      <c r="E22" t="s">
+        <v>227</v>
+      </c>
+      <c r="F22" t="s">
+        <v>227</v>
+      </c>
+      <c r="G22" t="s">
+        <v>128</v>
+      </c>
+      <c r="H22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22">
+        <v>0.984375</v>
+      </c>
+      <c r="J22">
+        <v>0.46441669633536498</v>
+      </c>
+      <c r="K22">
+        <v>3.5080687189961801</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M22" t="s">
+        <v>227</v>
+      </c>
+      <c r="N22" t="s">
+        <v>228</v>
+      </c>
+      <c r="O22">
+        <v>3.5080687189961801</v>
+      </c>
+      <c r="P22">
+        <v>1.60374934616561</v>
+      </c>
+      <c r="Q22">
+        <v>21</v>
+      </c>
+      <c r="R22">
+        <v>1.60374934616561</v>
+      </c>
+      <c r="S22">
+        <v>18</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" t="s">
+        <v>230</v>
+      </c>
+      <c r="D23" t="s">
+        <v>231</v>
+      </c>
+      <c r="E23" t="s">
+        <v>232</v>
+      </c>
+      <c r="F23" t="s">
+        <v>232</v>
+      </c>
+      <c r="G23" t="s">
+        <v>128</v>
+      </c>
+      <c r="H23" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0.39092718888665201</v>
+      </c>
+      <c r="K23">
+        <v>4.0288392120009497</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M23" t="s">
+        <v>232</v>
+      </c>
+      <c r="N23" t="s">
+        <v>233</v>
+      </c>
+      <c r="O23">
+        <v>4.0288392120009497</v>
+      </c>
+      <c r="P23">
+        <v>1.57498278762385</v>
+      </c>
+      <c r="Q23">
+        <v>22</v>
+      </c>
+      <c r="R23">
+        <v>1.57498278762385</v>
+      </c>
+      <c r="S23">
+        <v>19</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>234</v>
+      </c>
+      <c r="B24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" t="s">
+        <v>236</v>
+      </c>
+      <c r="E24" t="s">
+        <v>237</v>
+      </c>
+      <c r="F24" t="s">
+        <v>237</v>
+      </c>
+      <c r="G24" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24">
+        <v>0.96875</v>
+      </c>
+      <c r="J24">
+        <v>0.39555588746257703</v>
+      </c>
+      <c r="K24">
+        <v>3.5078059564292299</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M24" t="s">
+        <v>237</v>
+      </c>
+      <c r="N24" t="s">
+        <v>238</v>
+      </c>
+      <c r="O24">
+        <v>3.5078059564292299</v>
+      </c>
+      <c r="P24">
+        <v>1.3441728825749399</v>
+      </c>
+      <c r="Q24">
+        <v>23</v>
+      </c>
+      <c r="R24">
+        <v>1.3441728825749399</v>
+      </c>
+      <c r="S24">
+        <v>20</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" t="s">
+        <v>240</v>
+      </c>
+      <c r="D25" t="s">
+        <v>241</v>
+      </c>
+      <c r="E25" t="s">
+        <v>242</v>
+      </c>
+      <c r="F25" t="s">
+        <v>242</v>
+      </c>
+      <c r="G25" t="s">
+        <v>128</v>
+      </c>
+      <c r="H25" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25">
+        <v>0.953125</v>
+      </c>
+      <c r="J25">
+        <v>0.88923227106639702</v>
+      </c>
+      <c r="K25">
+        <v>1.5834845521536101</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M25" t="s">
+        <v>242</v>
+      </c>
+      <c r="N25" t="s">
+        <v>243</v>
+      </c>
+      <c r="O25">
+        <v>1.5834845521536101</v>
+      </c>
+      <c r="P25">
+        <v>1.3420815536737001</v>
+      </c>
+      <c r="Q25">
+        <v>24</v>
+      </c>
+      <c r="R25">
+        <v>1.9449904127305799</v>
+      </c>
+      <c r="S25">
+        <v>14</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>244</v>
+      </c>
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" t="s">
+        <v>245</v>
+      </c>
+      <c r="E26" t="s">
+        <v>246</v>
+      </c>
+      <c r="F26" t="s">
+        <v>246</v>
+      </c>
+      <c r="G26" t="s">
+        <v>128</v>
+      </c>
+      <c r="H26" t="s">
+        <v>129</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0.79646580105429099</v>
+      </c>
+      <c r="K26">
+        <v>1.68395906553816</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M26" t="s">
+        <v>246</v>
+      </c>
+      <c r="N26" t="s">
+        <v>247</v>
+      </c>
+      <c r="O26">
+        <v>1.68395906553816</v>
+      </c>
+      <c r="P26">
+        <v>1.3412158060764801</v>
+      </c>
+      <c r="Q26">
+        <v>25</v>
+      </c>
+      <c r="R26">
+        <v>10.112949522140299</v>
+      </c>
+      <c r="S26">
+        <v>2</v>
+      </c>
+      <c r="T26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>248</v>
+      </c>
+      <c r="B27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" t="s">
+        <v>249</v>
+      </c>
+      <c r="D27" t="s">
+        <v>250</v>
+      </c>
+      <c r="E27" t="s">
+        <v>251</v>
+      </c>
+      <c r="F27" t="s">
+        <v>251</v>
+      </c>
+      <c r="G27" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" t="s">
+        <v>129</v>
+      </c>
+      <c r="I27">
+        <v>0.96875</v>
+      </c>
+      <c r="J27">
+        <v>0.43047298917424098</v>
+      </c>
+      <c r="K27">
+        <v>3.0981736361377998</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M27" t="s">
+        <v>251</v>
+      </c>
+      <c r="N27" t="s">
+        <v>252</v>
+      </c>
+      <c r="O27">
+        <v>3.0981736361377998</v>
+      </c>
+      <c r="P27">
+        <v>1.2920025640625299</v>
+      </c>
+      <c r="Q27">
+        <v>26</v>
+      </c>
+      <c r="R27">
+        <v>1.2920025640625299</v>
+      </c>
+      <c r="S27">
+        <v>21</v>
+      </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>253</v>
+      </c>
+      <c r="B28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" t="s">
+        <v>254</v>
+      </c>
+      <c r="E28" t="s">
+        <v>255</v>
+      </c>
+      <c r="F28" t="s">
+        <v>255</v>
+      </c>
+      <c r="G28" t="s">
+        <v>128</v>
+      </c>
+      <c r="H28" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28">
+        <v>0.984375</v>
+      </c>
+      <c r="J28">
+        <v>0.33530226119738299</v>
+      </c>
+      <c r="K28">
+        <v>3.4166806774118101</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M28" t="s">
+        <v>255</v>
+      </c>
+      <c r="N28" t="s">
+        <v>256</v>
+      </c>
+      <c r="O28">
+        <v>3.4166806774118101</v>
+      </c>
+      <c r="P28">
+        <v>1.1277204325986201</v>
+      </c>
+      <c r="Q28">
+        <v>27</v>
+      </c>
+      <c r="R28">
+        <v>5.5567430041196104</v>
+      </c>
+      <c r="S28">
+        <v>5</v>
+      </c>
+      <c r="T28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>257</v>
+      </c>
+      <c r="B29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" t="s">
+        <v>258</v>
+      </c>
+      <c r="D29" t="s">
+        <v>259</v>
+      </c>
+      <c r="E29" t="s">
+        <v>260</v>
+      </c>
+      <c r="F29" t="s">
+        <v>260</v>
+      </c>
+      <c r="G29" t="s">
+        <v>128</v>
+      </c>
+      <c r="H29" t="s">
+        <v>129</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>4.8993442431853801E-2</v>
+      </c>
+      <c r="K29">
+        <v>16.509984484065399</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M29" t="s">
+        <v>260</v>
+      </c>
+      <c r="N29" t="s">
+        <v>261</v>
+      </c>
+      <c r="O29">
+        <v>16.509984484065399</v>
+      </c>
+      <c r="P29">
+        <v>0.80888097437085804</v>
+      </c>
+      <c r="Q29">
+        <v>28</v>
+      </c>
+      <c r="R29">
+        <v>0.80888097437085804</v>
+      </c>
+      <c r="S29">
+        <v>22</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>262</v>
+      </c>
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" t="s">
+        <v>263</v>
+      </c>
+      <c r="E30" t="s">
+        <v>264</v>
+      </c>
+      <c r="F30" t="s">
+        <v>264</v>
+      </c>
+      <c r="G30" t="s">
+        <v>128</v>
+      </c>
+      <c r="H30" t="s">
+        <v>129</v>
+      </c>
+      <c r="I30">
+        <v>0.953125</v>
+      </c>
+      <c r="J30">
+        <v>0.38173868650029502</v>
+      </c>
+      <c r="K30">
+        <v>1.95772561803939</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M30" t="s">
+        <v>264</v>
+      </c>
+      <c r="N30" t="s">
+        <v>265</v>
+      </c>
+      <c r="O30">
+        <v>1.95772561803939</v>
+      </c>
+      <c r="P30">
+        <v>0.71230806192904095</v>
+      </c>
+      <c r="Q30">
+        <v>29</v>
+      </c>
+      <c r="R30">
+        <v>10.112949522140299</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="T30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>266</v>
+      </c>
+      <c r="B31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" t="s">
+        <v>240</v>
+      </c>
+      <c r="D31" t="s">
+        <v>267</v>
+      </c>
+      <c r="E31" t="s">
+        <v>268</v>
+      </c>
+      <c r="F31" t="s">
+        <v>268</v>
+      </c>
+      <c r="G31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H31" t="s">
+        <v>129</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>0.62544784680397203</v>
+      </c>
+      <c r="K31">
+        <v>0.96396344177653703</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M31" t="s">
+        <v>268</v>
+      </c>
+      <c r="N31" t="s">
+        <v>269</v>
+      </c>
+      <c r="O31">
+        <v>0.96396344177653703</v>
+      </c>
+      <c r="P31">
+        <v>0.60290885905688096</v>
+      </c>
+      <c r="Q31">
+        <v>30</v>
+      </c>
+      <c r="R31">
+        <v>1.9449904127305799</v>
+      </c>
+      <c r="S31">
+        <v>14</v>
+      </c>
+      <c r="T31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>270</v>
+      </c>
+      <c r="B32" t="s">
+        <v>192</v>
+      </c>
+      <c r="C32" t="s">
+        <v>271</v>
+      </c>
+      <c r="D32" t="s">
+        <v>272</v>
+      </c>
+      <c r="E32" t="s">
+        <v>273</v>
+      </c>
+      <c r="F32" t="s">
+        <v>273</v>
+      </c>
+      <c r="G32" t="s">
+        <v>128</v>
+      </c>
+      <c r="H32" t="s">
+        <v>129</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>0.59116472031022704</v>
+      </c>
+      <c r="K32">
+        <v>0.96396344177653703</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M32" t="s">
+        <v>273</v>
+      </c>
+      <c r="N32" t="s">
+        <v>274</v>
+      </c>
+      <c r="O32">
+        <v>0.96396344177653703</v>
+      </c>
+      <c r="P32">
+        <v>0.56986117844711004</v>
+      </c>
+      <c r="Q32">
+        <v>31</v>
+      </c>
+      <c r="R32">
+        <v>0.56986117844711004</v>
+      </c>
+      <c r="S32">
+        <v>23</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" t="s">
+        <v>276</v>
+      </c>
+      <c r="D33" t="s">
+        <v>277</v>
+      </c>
+      <c r="E33" t="s">
+        <v>278</v>
+      </c>
+      <c r="F33" t="s">
+        <v>278</v>
+      </c>
+      <c r="G33" t="s">
+        <v>128</v>
+      </c>
+      <c r="H33" t="s">
+        <v>129</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>0.50526354006618601</v>
+      </c>
+      <c r="K33">
+        <v>0.87588169933499704</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M33" t="s">
+        <v>278</v>
+      </c>
+      <c r="N33" t="s">
+        <v>279</v>
+      </c>
+      <c r="O33">
+        <v>0.87588169933499704</v>
+      </c>
+      <c r="P33">
+        <v>0.44255108808518701</v>
+      </c>
+      <c r="Q33">
+        <v>32</v>
+      </c>
+      <c r="R33">
+        <v>0.44255108808518701</v>
+      </c>
+      <c r="S33">
+        <v>24</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>280</v>
+      </c>
+      <c r="B34" t="s">
+        <v>192</v>
+      </c>
+      <c r="C34" t="s">
+        <v>281</v>
+      </c>
+      <c r="D34" t="s">
+        <v>282</v>
+      </c>
+      <c r="E34" t="s">
+        <v>283</v>
+      </c>
+      <c r="F34" t="s">
+        <v>283</v>
+      </c>
+      <c r="G34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H34" t="s">
+        <v>129</v>
+      </c>
+      <c r="I34">
+        <v>0.890625</v>
+      </c>
+      <c r="J34">
+        <v>0.67802995928813703</v>
+      </c>
+      <c r="K34">
+        <v>0.55279096594409205</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M34" t="s">
+        <v>283</v>
+      </c>
+      <c r="N34" t="s">
+        <v>284</v>
+      </c>
+      <c r="O34">
+        <v>0.55279096594409205</v>
+      </c>
+      <c r="P34">
+        <v>0.33381411968177499</v>
+      </c>
+      <c r="Q34">
+        <v>33</v>
+      </c>
+      <c r="R34">
+        <v>0.372718370678084</v>
+      </c>
+      <c r="S34">
+        <v>25</v>
+      </c>
+      <c r="T34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>285</v>
+      </c>
+      <c r="B35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" t="s">
+        <v>286</v>
+      </c>
+      <c r="D35" t="s">
+        <v>287</v>
+      </c>
+      <c r="E35" t="s">
+        <v>288</v>
+      </c>
+      <c r="F35" t="s">
+        <v>288</v>
+      </c>
+      <c r="G35" t="s">
+        <v>128</v>
+      </c>
+      <c r="H35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I35">
+        <v>0.921875</v>
+      </c>
+      <c r="J35">
+        <v>0.38160818371930499</v>
+      </c>
+      <c r="K35">
+        <v>0.94237750815467503</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M35" t="s">
+        <v>288</v>
+      </c>
+      <c r="N35" t="s">
+        <v>289</v>
+      </c>
+      <c r="O35">
+        <v>0.94237750815467503</v>
+      </c>
+      <c r="P35">
+        <v>0.33152373729101597</v>
+      </c>
+      <c r="Q35">
+        <v>34</v>
+      </c>
+      <c r="R35">
+        <v>0.33152373729101597</v>
+      </c>
+      <c r="S35">
+        <v>26</v>
+      </c>
+      <c r="T35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>290</v>
+      </c>
+      <c r="B36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" t="s">
+        <v>291</v>
+      </c>
+      <c r="D36" t="s">
+        <v>292</v>
+      </c>
+      <c r="E36" t="s">
+        <v>293</v>
+      </c>
+      <c r="F36" t="s">
+        <v>293</v>
+      </c>
+      <c r="G36" t="s">
+        <v>128</v>
+      </c>
+      <c r="H36" t="s">
+        <v>129</v>
+      </c>
+      <c r="I36">
+        <v>0.9375</v>
+      </c>
+      <c r="J36">
+        <v>0.73911151576650302</v>
+      </c>
+      <c r="K36">
+        <v>0.39173166474141702</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M36" t="s">
+        <v>293</v>
+      </c>
+      <c r="N36" t="s">
+        <v>294</v>
+      </c>
+      <c r="O36">
+        <v>0.39173166474141702</v>
+      </c>
+      <c r="P36">
+        <v>0.27143754796946601</v>
+      </c>
+      <c r="Q36">
+        <v>35</v>
+      </c>
+      <c r="R36">
+        <v>0.32676796101977001</v>
+      </c>
+      <c r="S36">
+        <v>27</v>
+      </c>
+      <c r="T36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>295</v>
+      </c>
+      <c r="B37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" t="s">
+        <v>296</v>
+      </c>
+      <c r="D37" t="s">
+        <v>297</v>
+      </c>
+      <c r="E37" t="s">
+        <v>298</v>
+      </c>
+      <c r="F37" t="s">
+        <v>298</v>
+      </c>
+      <c r="G37" t="s">
+        <v>128</v>
+      </c>
+      <c r="H37" t="s">
+        <v>129</v>
+      </c>
+      <c r="I37">
+        <v>0.984375</v>
+      </c>
+      <c r="J37">
+        <v>0.39964569922424797</v>
+      </c>
+      <c r="K37">
+        <v>0.51368753102297304</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M37" t="s">
+        <v>298</v>
+      </c>
+      <c r="N37" t="s">
+        <v>299</v>
+      </c>
+      <c r="O37">
+        <v>0.51368753102297304</v>
+      </c>
+      <c r="P37">
+        <v>0.202085309197853</v>
+      </c>
+      <c r="Q37">
+        <v>36</v>
+      </c>
+      <c r="R37">
+        <v>0.202085309197853</v>
+      </c>
+      <c r="S37">
+        <v>28</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>300</v>
+      </c>
+      <c r="B38" t="s">
+        <v>192</v>
+      </c>
+      <c r="C38" t="s">
+        <v>301</v>
+      </c>
+      <c r="D38" t="s">
+        <v>302</v>
+      </c>
+      <c r="E38" t="s">
+        <v>303</v>
+      </c>
+      <c r="F38" t="s">
+        <v>303</v>
+      </c>
+      <c r="G38" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" t="s">
+        <v>129</v>
+      </c>
+      <c r="I38">
+        <v>0.96875</v>
+      </c>
+      <c r="J38">
+        <v>0.73629626361904998</v>
+      </c>
+      <c r="K38">
+        <v>0.211730293772459</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M38" t="s">
+        <v>303</v>
+      </c>
+      <c r="N38" t="s">
+        <v>304</v>
+      </c>
+      <c r="O38">
+        <v>0.211730293772459</v>
+      </c>
+      <c r="P38">
+        <v>0.151024467193387</v>
+      </c>
+      <c r="Q38">
+        <v>37</v>
+      </c>
+      <c r="R38">
+        <v>0.151024467193387</v>
+      </c>
+      <c r="S38">
+        <v>29</v>
+      </c>
+      <c r="T38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>305</v>
+      </c>
+      <c r="B39" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" t="s">
+        <v>306</v>
+      </c>
+      <c r="D39" t="s">
+        <v>307</v>
+      </c>
+      <c r="E39" t="s">
+        <v>308</v>
+      </c>
+      <c r="F39" t="s">
+        <v>308</v>
+      </c>
+      <c r="G39" t="s">
+        <v>128</v>
+      </c>
+      <c r="H39" t="s">
+        <v>129</v>
+      </c>
+      <c r="I39">
+        <v>0.96875</v>
+      </c>
+      <c r="J39">
+        <v>0.22554989675068501</v>
+      </c>
+      <c r="K39">
+        <v>0.41472077775032101</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M39" t="s">
+        <v>308</v>
+      </c>
+      <c r="N39" t="s">
+        <v>309</v>
+      </c>
+      <c r="O39">
+        <v>0.41472077775032101</v>
+      </c>
+      <c r="P39">
+        <v>9.0617096458137994E-2</v>
+      </c>
+      <c r="Q39">
+        <v>38</v>
+      </c>
+      <c r="R39">
+        <v>9.0617096458137994E-2</v>
+      </c>
+      <c r="S39">
+        <v>30</v>
+      </c>
+      <c r="T39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>310</v>
+      </c>
+      <c r="B40" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" t="s">
+        <v>311</v>
+      </c>
+      <c r="D40" t="s">
+        <v>312</v>
+      </c>
+      <c r="E40" t="s">
+        <v>313</v>
+      </c>
+      <c r="F40" t="s">
+        <v>313</v>
+      </c>
+      <c r="G40" t="s">
+        <v>128</v>
+      </c>
+      <c r="H40" t="s">
+        <v>129</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>0.91205195261698002</v>
+      </c>
+      <c r="K40">
+        <v>9.6886694557520095E-2</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M40" t="s">
+        <v>313</v>
+      </c>
+      <c r="N40" t="s">
+        <v>314</v>
+      </c>
+      <c r="O40">
+        <v>9.6886694557520095E-2</v>
+      </c>
+      <c r="P40">
+        <v>8.8365698953791094E-2</v>
+      </c>
+      <c r="Q40">
+        <v>39</v>
+      </c>
+      <c r="R40">
+        <v>8.8365698953791094E-2</v>
+      </c>
+      <c r="S40">
+        <v>31</v>
+      </c>
+      <c r="T40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>315</v>
+      </c>
+      <c r="B41" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" t="s">
+        <v>152</v>
+      </c>
+      <c r="D41" t="s">
+        <v>316</v>
+      </c>
+      <c r="E41" t="s">
+        <v>317</v>
+      </c>
+      <c r="F41" t="s">
+        <v>317</v>
+      </c>
+      <c r="G41" t="s">
+        <v>128</v>
+      </c>
+      <c r="H41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>0.26178273591996298</v>
+      </c>
+      <c r="K41">
+        <v>0.32345654994960799</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M41" t="s">
+        <v>317</v>
+      </c>
+      <c r="N41" t="s">
+        <v>318</v>
+      </c>
+      <c r="O41">
+        <v>0.32345654994960799</v>
+      </c>
+      <c r="P41">
+        <v>8.4675340597040696E-2</v>
+      </c>
+      <c r="Q41">
+        <v>40</v>
+      </c>
+      <c r="R41">
+        <v>10.112949522140299</v>
+      </c>
+      <c r="S41">
+        <v>2</v>
+      </c>
+      <c r="T41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>319</v>
+      </c>
+      <c r="B42" t="s">
+        <v>192</v>
+      </c>
+      <c r="C42" t="s">
+        <v>320</v>
+      </c>
+      <c r="D42" t="s">
+        <v>321</v>
+      </c>
+      <c r="E42" t="s">
+        <v>322</v>
+      </c>
+      <c r="F42" t="s">
+        <v>322</v>
+      </c>
+      <c r="G42" t="s">
+        <v>128</v>
+      </c>
+      <c r="H42" t="s">
+        <v>129</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>7.8017678783105504E-2</v>
+      </c>
+      <c r="K42">
+        <v>0.96396344177653703</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M42" t="s">
+        <v>322</v>
+      </c>
+      <c r="N42" t="s">
+        <v>323</v>
+      </c>
+      <c r="O42">
+        <v>0.96396344177653703</v>
+      </c>
+      <c r="P42">
+        <v>7.5206190159178704E-2</v>
+      </c>
+      <c r="Q42">
+        <v>41</v>
+      </c>
+      <c r="R42">
+        <v>7.5206190159178704E-2</v>
+      </c>
+      <c r="S42">
+        <v>32</v>
+      </c>
+      <c r="T42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>324</v>
+      </c>
+      <c r="B43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" t="s">
+        <v>325</v>
+      </c>
+      <c r="D43" t="s">
+        <v>326</v>
+      </c>
+      <c r="E43" t="s">
+        <v>327</v>
+      </c>
+      <c r="F43" t="s">
+        <v>327</v>
+      </c>
+      <c r="G43" t="s">
+        <v>174</v>
+      </c>
+      <c r="H43" t="s">
+        <v>129</v>
+      </c>
+      <c r="I43">
+        <v>0.90625</v>
+      </c>
+      <c r="J43">
+        <v>0.32070346747477402</v>
+      </c>
+      <c r="K43">
+        <v>0.211730293772459</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M43" t="s">
+        <v>327</v>
+      </c>
+      <c r="N43" t="s">
+        <v>328</v>
+      </c>
+      <c r="O43">
+        <v>0.211730293772459</v>
+      </c>
+      <c r="P43">
+        <v>6.1536766940191598E-2</v>
+      </c>
+      <c r="Q43">
+        <v>42</v>
+      </c>
+      <c r="R43">
+        <v>6.1536766940191598E-2</v>
+      </c>
+      <c r="S43">
+        <v>34</v>
+      </c>
+      <c r="T43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>329</v>
+      </c>
+      <c r="B44" t="s">
+        <v>192</v>
+      </c>
+      <c r="C44" t="s">
+        <v>330</v>
+      </c>
+      <c r="D44" t="s">
+        <v>331</v>
+      </c>
+      <c r="E44" t="s">
+        <v>332</v>
+      </c>
+      <c r="F44" t="s">
+        <v>332</v>
+      </c>
+      <c r="G44" t="s">
+        <v>128</v>
+      </c>
+      <c r="H44" t="s">
+        <v>129</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>0.19712707001949001</v>
+      </c>
+      <c r="K44">
+        <v>0.28878169697117301</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M44" t="s">
+        <v>332</v>
+      </c>
+      <c r="N44" t="s">
+        <v>333</v>
+      </c>
+      <c r="O44">
+        <v>0.28878169697117301</v>
+      </c>
+      <c r="P44">
+        <v>5.6926689799183701E-2</v>
+      </c>
+      <c r="Q44">
+        <v>43</v>
+      </c>
+      <c r="R44">
+        <v>5.6926689799183701E-2</v>
+      </c>
+      <c r="S44">
+        <v>35</v>
+      </c>
+      <c r="T44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>334</v>
+      </c>
+      <c r="B45" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" t="s">
+        <v>291</v>
+      </c>
+      <c r="D45" t="s">
+        <v>335</v>
+      </c>
+      <c r="E45" t="s">
+        <v>336</v>
+      </c>
+      <c r="F45" t="s">
+        <v>336</v>
+      </c>
+      <c r="G45" t="s">
+        <v>128</v>
+      </c>
+      <c r="H45" t="s">
+        <v>129</v>
+      </c>
+      <c r="I45">
+        <v>0.9375</v>
+      </c>
+      <c r="J45">
+        <v>0.21324255577110199</v>
+      </c>
+      <c r="K45">
+        <v>0.27676983630326002</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M45" t="s">
+        <v>336</v>
+      </c>
+      <c r="N45" t="s">
+        <v>337</v>
+      </c>
+      <c r="O45">
+        <v>0.27676983630326002</v>
+      </c>
+      <c r="P45">
+        <v>5.5330413050303402E-2</v>
+      </c>
+      <c r="Q45">
+        <v>44</v>
+      </c>
+      <c r="R45">
+        <v>0.32676796101977001</v>
+      </c>
+      <c r="S45">
+        <v>27</v>
+      </c>
+      <c r="T45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>338</v>
+      </c>
+      <c r="B46" t="s">
+        <v>192</v>
+      </c>
+      <c r="C46" t="s">
+        <v>339</v>
+      </c>
+      <c r="D46" t="s">
+        <v>340</v>
+      </c>
+      <c r="E46" t="s">
+        <v>341</v>
+      </c>
+      <c r="F46" t="s">
+        <v>341</v>
+      </c>
+      <c r="G46" t="s">
+        <v>128</v>
+      </c>
+      <c r="H46" t="s">
+        <v>129</v>
+      </c>
+      <c r="I46">
+        <v>0.984375</v>
+      </c>
+      <c r="J46">
+        <v>2.9606465221766E-2</v>
+      </c>
+      <c r="K46">
+        <v>1.64944790305443</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M46" t="s">
+        <v>341</v>
+      </c>
+      <c r="N46" t="s">
+        <v>342</v>
+      </c>
+      <c r="O46">
+        <v>1.64944790305443</v>
+      </c>
+      <c r="P46">
+        <v>4.8071285696006903E-2</v>
+      </c>
+      <c r="Q46">
+        <v>45</v>
+      </c>
+      <c r="R46">
+        <v>6.6996583458947101E-2</v>
+      </c>
+      <c r="S46">
+        <v>33</v>
+      </c>
+      <c r="T46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>343</v>
+      </c>
+      <c r="B47" t="s">
+        <v>192</v>
+      </c>
+      <c r="C47" t="s">
+        <v>281</v>
+      </c>
+      <c r="D47" t="s">
+        <v>344</v>
+      </c>
+      <c r="E47" t="s">
+        <v>345</v>
+      </c>
+      <c r="F47" t="s">
+        <v>345</v>
+      </c>
+      <c r="G47" t="s">
+        <v>128</v>
+      </c>
+      <c r="H47" t="s">
+        <v>129</v>
+      </c>
+      <c r="I47">
+        <v>0.921875</v>
+      </c>
+      <c r="J47">
+        <v>0.17132320465824699</v>
+      </c>
+      <c r="K47">
+        <v>0.246325192806821</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M47" t="s">
+        <v>345</v>
+      </c>
+      <c r="N47" t="s">
+        <v>346</v>
+      </c>
+      <c r="O47">
+        <v>0.246325192806821</v>
+      </c>
+      <c r="P47">
+        <v>3.8904250996309203E-2</v>
+      </c>
+      <c r="Q47">
+        <v>46</v>
+      </c>
+      <c r="R47">
+        <v>0.372718370678084</v>
+      </c>
+      <c r="S47">
+        <v>25</v>
+      </c>
+      <c r="T47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>347</v>
+      </c>
+      <c r="B48" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48" t="s">
+        <v>348</v>
+      </c>
+      <c r="E48" t="s">
+        <v>349</v>
+      </c>
+      <c r="F48" t="s">
+        <v>349</v>
+      </c>
+      <c r="G48" t="s">
+        <v>128</v>
+      </c>
+      <c r="H48" t="s">
+        <v>129</v>
+      </c>
+      <c r="I48">
+        <v>0.984375</v>
+      </c>
+      <c r="J48">
+        <v>0.74943401415274002</v>
+      </c>
+      <c r="K48">
+        <v>3.3756212394582201E-2</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M48" t="s">
+        <v>349</v>
+      </c>
+      <c r="N48" t="s">
+        <v>350</v>
+      </c>
+      <c r="O48">
+        <v>3.3756212394582201E-2</v>
+      </c>
+      <c r="P48">
+        <v>2.4902771667503799E-2</v>
+      </c>
+      <c r="Q48">
+        <v>47</v>
+      </c>
+      <c r="R48">
+        <v>10.112949522140299</v>
+      </c>
+      <c r="S48">
+        <v>2</v>
+      </c>
+      <c r="T48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>351</v>
+      </c>
+      <c r="B49" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" t="s">
+        <v>352</v>
+      </c>
+      <c r="D49" t="s">
+        <v>353</v>
+      </c>
+      <c r="E49" t="s">
+        <v>354</v>
+      </c>
+      <c r="F49" t="s">
+        <v>354</v>
+      </c>
+      <c r="G49" t="s">
+        <v>128</v>
+      </c>
+      <c r="H49" t="s">
+        <v>129</v>
+      </c>
+      <c r="I49">
+        <v>0.84375</v>
+      </c>
+      <c r="J49">
+        <v>0.72342010515549404</v>
+      </c>
+      <c r="K49">
+        <v>4.0602340114072898E-2</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M49" t="s">
+        <v>354</v>
+      </c>
+      <c r="N49" t="s">
+        <v>355</v>
+      </c>
+      <c r="O49">
+        <v>4.0602340114072898E-2</v>
+      </c>
+      <c r="P49">
+        <v>2.4783088349431499E-2</v>
+      </c>
+      <c r="Q49">
+        <v>48</v>
+      </c>
+      <c r="R49">
+        <v>2.4783088349431499E-2</v>
+      </c>
+      <c r="S49">
+        <v>36</v>
+      </c>
+      <c r="T49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>356</v>
+      </c>
+      <c r="B50" t="s">
+        <v>192</v>
+      </c>
+      <c r="C50" t="s">
+        <v>357</v>
+      </c>
+      <c r="D50" t="s">
+        <v>358</v>
+      </c>
+      <c r="E50" t="s">
+        <v>359</v>
+      </c>
+      <c r="F50" t="s">
+        <v>359</v>
+      </c>
+      <c r="G50" t="s">
+        <v>128</v>
+      </c>
+      <c r="H50" t="s">
+        <v>129</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>0.13485842710367099</v>
+      </c>
+      <c r="K50">
+        <v>0.154126447150124</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M50" t="s">
+        <v>359</v>
+      </c>
+      <c r="N50" t="s">
+        <v>360</v>
+      </c>
+      <c r="O50">
+        <v>0.154126447150124</v>
+      </c>
+      <c r="P50">
+        <v>2.0785250237742799E-2</v>
+      </c>
+      <c r="Q50">
+        <v>49</v>
+      </c>
+      <c r="R50">
+        <v>2.0785250237742799E-2</v>
+      </c>
+      <c r="S50">
+        <v>37</v>
+      </c>
+      <c r="T50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>361</v>
+      </c>
+      <c r="B51" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" t="s">
+        <v>339</v>
+      </c>
+      <c r="D51" t="s">
+        <v>362</v>
+      </c>
+      <c r="E51" t="s">
+        <v>363</v>
+      </c>
+      <c r="F51" t="s">
+        <v>363</v>
+      </c>
+      <c r="G51" t="s">
+        <v>128</v>
+      </c>
+      <c r="H51" t="s">
+        <v>129</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>4.7185036935701004E-3</v>
+      </c>
+      <c r="K51">
+        <v>4.01086848543315</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="M51" t="s">
+        <v>363</v>
+      </c>
+      <c r="N51" t="s">
+        <v>364</v>
+      </c>
+      <c r="O51">
+        <v>4.01086848543315</v>
+      </c>
+      <c r="P51">
+        <v>1.8925297762940201E-2</v>
+      </c>
+      <c r="Q51">
+        <v>50</v>
+      </c>
+      <c r="R51">
+        <v>6.6996583458947101E-2</v>
+      </c>
+      <c r="S51">
+        <v>33</v>
+      </c>
+      <c r="T51">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E60D12-1FDF-E140-945D-8437118D68CC}">
   <dimension ref="A1:S16"/>
   <sheetViews>

</xml_diff>